<commit_message>
feat: preserve header formatting; duplicate numeric tool items supported; web zip named as job folder; template updates
</commit_message>
<xml_diff>
--- a/templates/F-825-1032F CMD-J.L00.00.C aprevo TLIF-CA Fnl QC Insp.xlsx
+++ b/templates/F-825-1032F CMD-J.L00.00.C aprevo TLIF-CA Fnl QC Insp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AI Records\Empty Templates\Fake 825\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Nguyen\Desktop\Compare 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ADCAEE-8092-475C-A421-BC0BC350863C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F703218-55BA-4D44-8B88-40340488C4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,9 +340,6 @@
     <t>{{Item 6}}</t>
   </si>
   <si>
-    <t>{{Item 7}}</t>
-  </si>
-  <si>
     <t>{{Item 8}}</t>
   </si>
   <si>
@@ -377,13 +374,16 @@
   </si>
   <si>
     <t>{{Job Number}}</t>
+  </si>
+  <si>
+    <t>{{Item7}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,12 +418,6 @@
     </font>
     <font>
       <i/>
-      <sz val="8"/>
-      <color rgb="FF0070C0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF0070C0"/>
       <name val="Aptos Narrow"/>
@@ -723,7 +717,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -800,9 +794,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -819,33 +810,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -876,6 +840,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -896,9 +863,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -914,19 +878,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -953,10 +917,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -986,25 +950,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1340,7 +1334,7 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:D12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="11.7" x14ac:dyDescent="0.45"/>
@@ -1355,250 +1349,250 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="103" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="92" t="s">
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="94" t="s">
+      <c r="J1" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="95"/>
-      <c r="L1" s="96"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="86"/>
     </row>
     <row r="2" spans="1:12" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
-      <c r="A2" s="75"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="99"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="89"/>
     </row>
     <row r="3" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="99" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="101" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="102"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="102"/>
+      <c r="L3" s="103"/>
+    </row>
+    <row r="4" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" s="49"/>
-      <c r="L3" s="50"/>
-    </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="41" t="s">
+      <c r="D4" s="99" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="48"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="106"/>
+    </row>
+    <row r="5" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D5" s="99" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="48"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="106"/>
+    </row>
+    <row r="6" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="53"/>
-    </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="41" t="s">
+      <c r="D6" s="99" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="48"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="106"/>
+    </row>
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D7" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="48"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="104"/>
+      <c r="K7" s="105"/>
+      <c r="L7" s="106"/>
+    </row>
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="53"/>
-    </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="41" t="s">
+      <c r="D8" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="48"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="106"/>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="48"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="106"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="106"/>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="43"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D10" s="99" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="45"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
-    </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="44"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="53"/>
-    </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="53"/>
-    </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="E9" s="58"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="53"/>
-    </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="53"/>
-    </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="41" t="s">
+      <c r="D11" s="99" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="E11" s="49"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="108"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="108"/>
+      <c r="L11" s="109"/>
+    </row>
+    <row r="12" spans="1:12" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A12" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="65"/>
+      <c r="C12" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="59"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="56"/>
-    </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="75" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="109" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="109"/>
+      <c r="D12" s="100"/>
       <c r="E12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="100"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="102"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="92"/>
       <c r="I12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="100"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="102"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="92"/>
     </row>
     <row r="13" spans="1:12" s="6" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="78"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="81"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="71"/>
     </row>
     <row r="14" spans="1:12" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="15" spans="1:12" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -1629,11 +1623,11 @@
       <c r="I15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="75" t="s">
+      <c r="J15" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="75"/>
-      <c r="L15" s="75"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
     </row>
     <row r="16" spans="1:12" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
@@ -1659,11 +1653,11 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="66" t="s">
+      <c r="J16" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
     </row>
     <row r="17" spans="1:12" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
@@ -1689,11 +1683,11 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="66" t="s">
+      <c r="J17" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
     </row>
     <row r="18" spans="1:12" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
@@ -1719,11 +1713,11 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="66" t="s">
+      <c r="J18" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="66"/>
-      <c r="L18" s="66"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
     </row>
     <row r="19" spans="1:12" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
@@ -1749,11 +1743,11 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="66" t="s">
+      <c r="J19" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="66"/>
-      <c r="L19" s="66"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
     </row>
     <row r="20" spans="1:12" s="6" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
@@ -1779,11 +1773,11 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="66" t="s">
+      <c r="J20" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="66"/>
-      <c r="L20" s="66"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
     </row>
     <row r="21" spans="1:12" s="6" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
@@ -1809,11 +1803,11 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="66" t="s">
+      <c r="J21" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K21" s="66"/>
-      <c r="L21" s="66"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
     </row>
     <row r="22" spans="1:12" s="6" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
@@ -1839,11 +1833,11 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="66" t="s">
+      <c r="J22" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K22" s="66"/>
-      <c r="L22" s="66"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
     </row>
     <row r="23" spans="1:12" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
@@ -1869,11 +1863,11 @@
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="66" t="s">
+      <c r="J23" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="66"/>
-      <c r="L23" s="66"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
     </row>
     <row r="24" spans="1:12" s="6" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
@@ -1899,11 +1893,11 @@
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
-      <c r="J24" s="73" t="s">
+      <c r="J24" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
     </row>
     <row r="25" spans="1:12" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
@@ -1929,11 +1923,11 @@
       </c>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
-      <c r="J25" s="73" t="s">
+      <c r="J25" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
     </row>
     <row r="26" spans="1:12" s="32" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
@@ -1959,11 +1953,11 @@
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="73" t="s">
+      <c r="J26" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
     </row>
     <row r="27" spans="1:12" s="6" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
@@ -1989,53 +1983,53 @@
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="73" t="s">
+      <c r="J27" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="K27" s="73"/>
-      <c r="L27" s="73"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
     </row>
     <row r="28" spans="1:12" s="6" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="33"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="61"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="51"/>
     </row>
     <row r="29" spans="1:12" s="6" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="34"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="62"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="63"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="53"/>
     </row>
     <row r="30" spans="1:12" s="6" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="35"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="65"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="55"/>
     </row>
     <row r="31" spans="1:12" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4"/>
     <row r="32" spans="1:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
@@ -2048,25 +2042,25 @@
       <c r="D32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="84" t="s">
+      <c r="F32" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="84" t="s">
+      <c r="G32" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="57" t="s">
+      <c r="H32" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="57" t="s">
+      <c r="I32" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="J32" s="57" t="s">
+      <c r="J32" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="K32" s="57" t="s">
+      <c r="K32" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="L32" s="57" t="s">
+      <c r="L32" s="47" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2076,13 +2070,13 @@
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="13"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="85"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="59"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="59"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
     </row>
     <row r="34" spans="2:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B34" s="12" t="s">
@@ -2090,25 +2084,25 @@
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="13"/>
-      <c r="F34" s="82" t="s">
+      <c r="F34" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="88">
+      <c r="G34" s="78">
         <v>1</v>
       </c>
-      <c r="H34" s="90">
+      <c r="H34" s="80">
         <v>8</v>
       </c>
-      <c r="I34" s="90">
+      <c r="I34" s="80">
         <v>12</v>
       </c>
-      <c r="J34" s="90">
+      <c r="J34" s="80">
         <v>19</v>
       </c>
-      <c r="K34" s="90">
+      <c r="K34" s="80">
         <v>21</v>
       </c>
-      <c r="L34" s="86" t="s">
+      <c r="L34" s="76" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2116,13 +2110,13 @@
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="13"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="91"/>
-      <c r="I35" s="91"/>
-      <c r="J35" s="91"/>
-      <c r="K35" s="91"/>
-      <c r="L35" s="87"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="77"/>
     </row>
     <row r="36" spans="2:12" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="12"/>
@@ -2130,15 +2124,15 @@
       <c r="D36" s="13"/>
     </row>
     <row r="37" spans="2:12" s="6" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F37" s="74" t="s">
+      <c r="F37" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="G37" s="74"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="64"/>
+      <c r="J37" s="64"/>
+      <c r="K37" s="64"/>
+      <c r="L37" s="64"/>
     </row>
     <row r="38" spans="2:12" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
       <c r="F38" s="21"/>
@@ -2195,16 +2189,16 @@
       <c r="D46" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E46" s="67" t="s">
+      <c r="E46" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="68"/>
-      <c r="G46" s="68"/>
-      <c r="H46" s="68"/>
-      <c r="I46" s="68"/>
-      <c r="J46" s="68"/>
-      <c r="K46" s="68"/>
-      <c r="L46" s="68"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
+      <c r="J46" s="59"/>
+      <c r="K46" s="59"/>
+      <c r="L46" s="59"/>
     </row>
     <row r="47" spans="2:12" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
       <c r="B47" s="1" t="s">
@@ -2216,16 +2210,16 @@
       <c r="D47" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="69" t="s">
+      <c r="E47" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="70"/>
-      <c r="L47" s="70"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="61"/>
+      <c r="L47" s="61"/>
     </row>
     <row r="48" spans="2:12" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
       <c r="B48" s="8"/>
@@ -2249,16 +2243,16 @@
       <c r="D50" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E50" s="71" t="s">
+      <c r="E50" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="F50" s="72"/>
-      <c r="G50" s="72"/>
-      <c r="H50" s="72"/>
-      <c r="I50" s="72"/>
-      <c r="J50" s="72"/>
-      <c r="K50" s="72"/>
-      <c r="L50" s="72"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="63"/>
+      <c r="J50" s="63"/>
+      <c r="K50" s="63"/>
+      <c r="L50" s="63"/>
     </row>
     <row r="51" spans="2:12" s="6" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" s="1" t="s">
@@ -2270,16 +2264,16 @@
       <c r="D51" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E51" s="73" t="s">
+      <c r="E51" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="F51" s="73"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="73"/>
-      <c r="I51" s="73"/>
-      <c r="J51" s="73"/>
-      <c r="K51" s="73"/>
-      <c r="L51" s="73"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
     </row>
     <row r="52" spans="2:12" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
       <c r="B52" s="1" t="s">
@@ -2291,16 +2285,16 @@
       <c r="D52" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="66" t="s">
+      <c r="E52" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="F52" s="66"/>
-      <c r="G52" s="66"/>
-      <c r="H52" s="66"/>
-      <c r="I52" s="66"/>
-      <c r="J52" s="66"/>
-      <c r="K52" s="66"/>
-      <c r="L52" s="66"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="57"/>
     </row>
     <row r="53" spans="2:12" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
       <c r="B53" s="1" t="s">
@@ -2312,16 +2306,16 @@
       <c r="D53" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E53" s="66" t="s">
+      <c r="E53" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="F53" s="66"/>
-      <c r="G53" s="66"/>
-      <c r="H53" s="66"/>
-      <c r="I53" s="66"/>
-      <c r="J53" s="66"/>
-      <c r="K53" s="66"/>
-      <c r="L53" s="66"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="57"/>
+      <c r="J53" s="57"/>
+      <c r="K53" s="57"/>
+      <c r="L53" s="57"/>
     </row>
     <row r="54" spans="2:12" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4"/>
     <row r="55" spans="2:12" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4"/>
@@ -2379,7 +2373,7 @@
     <mergeCell ref="J21:L21"/>
     <mergeCell ref="J22:L22"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.4" right="0.4" top="1" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -2816,7 +2810,7 @@
     <row r="66" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="67" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.4" right="0.4" top="1" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>